<commit_message>
Starting "Environmental Vision" Functioanlity
</commit_message>
<xml_diff>
--- a/docs/gantt/Gantt Chart_2.xlsx
+++ b/docs/gantt/Gantt Chart_2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Software Engineering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KeyStone\docs\gantt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5453B657-2736-4DB9-A22C-FAEBDF0329FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D368AC-BB35-4B7A-BBF8-F08E4FD21C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="70">
   <si>
     <t>GANTT CHART</t>
   </si>
@@ -334,6 +334,9 @@
   </si>
   <si>
     <t>2/30/2022</t>
+  </si>
+  <si>
+    <t>Environmental Vision</t>
   </si>
 </sst>
 </file>
@@ -1100,14 +1103,46 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="27" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1118,25 +1153,12 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1147,25 +1169,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="27" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1532,24 +1535,24 @@
     <tabColor rgb="FF3D85C6"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BY38"/>
+  <dimension ref="A1:BY39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AL31" sqref="AL31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="38.21875" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="38.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
     <col min="5" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" customWidth="1"/>
-    <col min="8" max="77" width="3.44140625" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="8" max="77" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:77" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1628,39 +1631,39 @@
       <c r="BX1" s="1"/>
       <c r="BY1" s="1"/>
     </row>
-    <row r="2" spans="1:77" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:77" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="87" t="s">
+      <c r="B2" s="101" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="90"/>
-      <c r="O2" s="88"/>
-      <c r="P2" s="88"/>
-      <c r="Q2" s="88"/>
-      <c r="R2" s="88"/>
-      <c r="S2" s="88"/>
-      <c r="T2" s="88"/>
-      <c r="U2" s="88"/>
-      <c r="V2" s="88"/>
-      <c r="W2" s="88"/>
-      <c r="X2" s="88"/>
-      <c r="Y2" s="88"/>
-      <c r="Z2" s="88"/>
-      <c r="AA2" s="88"/>
-      <c r="AB2" s="88"/>
-      <c r="AC2" s="88"/>
-      <c r="AD2" s="88"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="102"/>
+      <c r="M2" s="102"/>
+      <c r="N2" s="104"/>
+      <c r="O2" s="102"/>
+      <c r="P2" s="102"/>
+      <c r="Q2" s="102"/>
+      <c r="R2" s="102"/>
+      <c r="S2" s="102"/>
+      <c r="T2" s="102"/>
+      <c r="U2" s="102"/>
+      <c r="V2" s="102"/>
+      <c r="W2" s="102"/>
+      <c r="X2" s="102"/>
+      <c r="Y2" s="102"/>
+      <c r="Z2" s="102"/>
+      <c r="AA2" s="102"/>
+      <c r="AB2" s="102"/>
+      <c r="AC2" s="102"/>
+      <c r="AD2" s="102"/>
       <c r="AE2" s="11"/>
       <c r="AF2" s="11"/>
       <c r="AG2" s="11"/>
@@ -1709,7 +1712,7 @@
       <c r="BX2" s="1"/>
       <c r="BY2" s="1"/>
     </row>
-    <row r="3" spans="1:77" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:77" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -1788,42 +1791,42 @@
       <c r="BX3" s="1"/>
       <c r="BY3" s="1"/>
     </row>
-    <row r="4" spans="1:77" ht="21" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:77" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1"/>
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="92"/>
-      <c r="D4" s="93" t="s">
+      <c r="C4" s="88"/>
+      <c r="D4" s="105" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="94"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="91" t="s">
+      <c r="E4" s="90"/>
+      <c r="F4" s="90"/>
+      <c r="G4" s="90"/>
+      <c r="H4" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="92"/>
-      <c r="J4" s="92"/>
-      <c r="K4" s="92"/>
-      <c r="L4" s="92"/>
-      <c r="M4" s="92"/>
-      <c r="N4" s="92"/>
-      <c r="O4" s="95" t="s">
+      <c r="I4" s="88"/>
+      <c r="J4" s="88"/>
+      <c r="K4" s="88"/>
+      <c r="L4" s="88"/>
+      <c r="M4" s="88"/>
+      <c r="N4" s="88"/>
+      <c r="O4" s="106" t="s">
         <v>2</v>
       </c>
-      <c r="P4" s="94"/>
-      <c r="Q4" s="94"/>
-      <c r="R4" s="94"/>
-      <c r="S4" s="94"/>
-      <c r="T4" s="94"/>
-      <c r="U4" s="94"/>
-      <c r="V4" s="94"/>
-      <c r="W4" s="94"/>
-      <c r="X4" s="94"/>
-      <c r="Y4" s="94"/>
-      <c r="Z4" s="94"/>
-      <c r="AA4" s="94"/>
+      <c r="P4" s="90"/>
+      <c r="Q4" s="90"/>
+      <c r="R4" s="90"/>
+      <c r="S4" s="90"/>
+      <c r="T4" s="90"/>
+      <c r="U4" s="90"/>
+      <c r="V4" s="90"/>
+      <c r="W4" s="90"/>
+      <c r="X4" s="90"/>
+      <c r="Y4" s="90"/>
+      <c r="Z4" s="90"/>
+      <c r="AA4" s="90"/>
       <c r="AB4" s="16"/>
       <c r="AC4" s="10"/>
       <c r="AD4" s="10"/>
@@ -1875,41 +1878,41 @@
       <c r="BX4" s="1"/>
       <c r="BY4" s="1"/>
     </row>
-    <row r="5" spans="1:77" ht="21" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:77" ht="21" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A5" s="1"/>
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="92"/>
-      <c r="D5" s="105" t="s">
+      <c r="C5" s="88"/>
+      <c r="D5" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="94"/>
-      <c r="F5" s="94"/>
-      <c r="G5" s="94"/>
-      <c r="H5" s="91" t="s">
+      <c r="E5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="90"/>
+      <c r="H5" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="92"/>
-      <c r="J5" s="92"/>
-      <c r="K5" s="92"/>
-      <c r="L5" s="92"/>
-      <c r="M5" s="92"/>
-      <c r="N5" s="92"/>
-      <c r="O5" s="106">
+      <c r="I5" s="88"/>
+      <c r="J5" s="88"/>
+      <c r="K5" s="88"/>
+      <c r="L5" s="88"/>
+      <c r="M5" s="88"/>
+      <c r="N5" s="88"/>
+      <c r="O5" s="91">
         <v>44596</v>
       </c>
-      <c r="P5" s="94"/>
-      <c r="Q5" s="94"/>
-      <c r="R5" s="94"/>
-      <c r="S5" s="94"/>
-      <c r="T5" s="94"/>
-      <c r="U5" s="94"/>
-      <c r="V5" s="94"/>
-      <c r="W5" s="94"/>
-      <c r="X5" s="94"/>
-      <c r="Y5" s="94"/>
-      <c r="Z5" s="94"/>
+      <c r="P5" s="90"/>
+      <c r="Q5" s="90"/>
+      <c r="R5" s="90"/>
+      <c r="S5" s="90"/>
+      <c r="T5" s="90"/>
+      <c r="U5" s="90"/>
+      <c r="V5" s="90"/>
+      <c r="W5" s="90"/>
+      <c r="X5" s="90"/>
+      <c r="Y5" s="90"/>
+      <c r="Z5" s="90"/>
       <c r="AA5" s="17"/>
       <c r="AB5" s="16"/>
       <c r="AC5" s="1"/>
@@ -1962,12 +1965,12 @@
       <c r="BX5" s="1"/>
       <c r="BY5" s="1"/>
     </row>
-    <row r="6" spans="1:77" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:77" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="19"/>
-      <c r="B6" s="91" t="s">
+      <c r="B6" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="92"/>
+      <c r="C6" s="88"/>
       <c r="D6" s="49" t="s">
         <v>20</v>
       </c>
@@ -1982,14 +1985,14 @@
       <c r="M6" s="19"/>
       <c r="N6" s="19"/>
       <c r="O6" s="65"/>
-      <c r="P6" s="101" t="s">
+      <c r="P6" s="108" t="s">
         <v>51</v>
       </c>
-      <c r="Q6" s="101"/>
-      <c r="R6" s="101"/>
-      <c r="S6" s="101"/>
-      <c r="T6" s="101"/>
-      <c r="U6" s="101"/>
+      <c r="Q6" s="108"/>
+      <c r="R6" s="108"/>
+      <c r="S6" s="108"/>
+      <c r="T6" s="108"/>
+      <c r="U6" s="108"/>
       <c r="V6" s="19"/>
       <c r="W6" s="19"/>
       <c r="X6" s="19"/>
@@ -2047,34 +2050,34 @@
       <c r="BX6" s="19"/>
       <c r="BY6" s="19"/>
     </row>
-    <row r="7" spans="1:77" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:77" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="19"/>
-      <c r="B7" s="91" t="s">
+      <c r="B7" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="92"/>
-      <c r="D7" s="100" t="s">
+      <c r="C7" s="88"/>
+      <c r="D7" s="107" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="100"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="100"/>
-      <c r="H7" s="100"/>
-      <c r="I7" s="100"/>
-      <c r="J7" s="100"/>
-      <c r="K7" s="100"/>
-      <c r="L7" s="100"/>
-      <c r="M7" s="100"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="107"/>
+      <c r="G7" s="107"/>
+      <c r="H7" s="107"/>
+      <c r="I7" s="107"/>
+      <c r="J7" s="107"/>
+      <c r="K7" s="107"/>
+      <c r="L7" s="107"/>
+      <c r="M7" s="107"/>
       <c r="N7" s="19"/>
       <c r="O7" s="66"/>
-      <c r="P7" s="103" t="s">
+      <c r="P7" s="110" t="s">
         <v>49</v>
       </c>
-      <c r="Q7" s="103"/>
-      <c r="R7" s="103"/>
-      <c r="S7" s="103"/>
-      <c r="T7" s="103"/>
-      <c r="U7" s="103"/>
+      <c r="Q7" s="110"/>
+      <c r="R7" s="110"/>
+      <c r="S7" s="110"/>
+      <c r="T7" s="110"/>
+      <c r="U7" s="110"/>
       <c r="V7" s="19"/>
       <c r="W7" s="19"/>
       <c r="X7" s="19"/>
@@ -2132,220 +2135,220 @@
       <c r="BX7" s="19"/>
       <c r="BY7" s="19"/>
     </row>
-    <row r="8" spans="1:77" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:77" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="O8" s="67"/>
-      <c r="P8" s="102" t="s">
+      <c r="P8" s="109" t="s">
         <v>50</v>
       </c>
-      <c r="Q8" s="102"/>
-      <c r="R8" s="102"/>
-      <c r="S8" s="102"/>
-      <c r="T8" s="102"/>
-      <c r="U8" s="102"/>
+      <c r="Q8" s="109"/>
+      <c r="R8" s="109"/>
+      <c r="S8" s="109"/>
+      <c r="T8" s="109"/>
+      <c r="U8" s="109"/>
     </row>
-    <row r="9" spans="1:77" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:77" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="23"/>
     </row>
-    <row r="10" spans="1:77" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:77" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="19"/>
-      <c r="B10" s="83" t="s">
+      <c r="B10" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="83" t="s">
+      <c r="C10" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="83" t="s">
+      <c r="D10" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="83" t="s">
+      <c r="E10" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="83" t="s">
+      <c r="F10" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="83" t="s">
+      <c r="G10" s="92" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="85"/>
-      <c r="I10" s="86"/>
-      <c r="J10" s="86"/>
-      <c r="K10" s="86"/>
-      <c r="L10" s="86"/>
-      <c r="M10" s="86"/>
-      <c r="N10" s="86"/>
-      <c r="O10" s="86"/>
-      <c r="P10" s="86"/>
-      <c r="Q10" s="86"/>
-      <c r="R10" s="86"/>
-      <c r="S10" s="86"/>
-      <c r="T10" s="86"/>
-      <c r="U10" s="86"/>
-      <c r="V10" s="86"/>
-      <c r="W10" s="96"/>
-      <c r="X10" s="86"/>
-      <c r="Y10" s="86"/>
-      <c r="Z10" s="86"/>
-      <c r="AA10" s="86"/>
-      <c r="AB10" s="86"/>
-      <c r="AC10" s="86"/>
-      <c r="AD10" s="86"/>
-      <c r="AE10" s="86"/>
-      <c r="AF10" s="86"/>
-      <c r="AG10" s="86"/>
-      <c r="AH10" s="86"/>
-      <c r="AI10" s="86"/>
-      <c r="AJ10" s="86"/>
-      <c r="AK10" s="86"/>
-      <c r="AL10" s="96"/>
-      <c r="AM10" s="86"/>
-      <c r="AN10" s="86"/>
-      <c r="AO10" s="86"/>
-      <c r="AP10" s="86"/>
-      <c r="AQ10" s="86"/>
-      <c r="AR10" s="86"/>
-      <c r="AS10" s="86"/>
-      <c r="AT10" s="86"/>
-      <c r="AU10" s="86"/>
-      <c r="AV10" s="86"/>
-      <c r="AW10" s="86"/>
-      <c r="AX10" s="86"/>
-      <c r="AY10" s="86"/>
-      <c r="AZ10" s="86"/>
-      <c r="BA10" s="96"/>
-      <c r="BB10" s="86"/>
-      <c r="BC10" s="86"/>
-      <c r="BD10" s="86"/>
-      <c r="BE10" s="86"/>
-      <c r="BF10" s="86"/>
-      <c r="BG10" s="86"/>
-      <c r="BH10" s="86"/>
-      <c r="BI10" s="86"/>
-      <c r="BJ10" s="86"/>
-      <c r="BK10" s="86"/>
-      <c r="BL10" s="86"/>
-      <c r="BM10" s="86"/>
-      <c r="BN10" s="86"/>
-      <c r="BO10" s="86"/>
-      <c r="BP10" s="86"/>
-      <c r="BQ10" s="86"/>
-      <c r="BR10" s="86"/>
-      <c r="BS10" s="86"/>
-      <c r="BT10" s="86"/>
-      <c r="BU10" s="86"/>
-      <c r="BV10" s="86"/>
-      <c r="BW10" s="86"/>
-      <c r="BX10" s="86"/>
-      <c r="BY10" s="104"/>
+      <c r="H10" s="100"/>
+      <c r="I10" s="98"/>
+      <c r="J10" s="98"/>
+      <c r="K10" s="98"/>
+      <c r="L10" s="98"/>
+      <c r="M10" s="98"/>
+      <c r="N10" s="98"/>
+      <c r="O10" s="98"/>
+      <c r="P10" s="98"/>
+      <c r="Q10" s="98"/>
+      <c r="R10" s="98"/>
+      <c r="S10" s="98"/>
+      <c r="T10" s="98"/>
+      <c r="U10" s="98"/>
+      <c r="V10" s="98"/>
+      <c r="W10" s="97"/>
+      <c r="X10" s="98"/>
+      <c r="Y10" s="98"/>
+      <c r="Z10" s="98"/>
+      <c r="AA10" s="98"/>
+      <c r="AB10" s="98"/>
+      <c r="AC10" s="98"/>
+      <c r="AD10" s="98"/>
+      <c r="AE10" s="98"/>
+      <c r="AF10" s="98"/>
+      <c r="AG10" s="98"/>
+      <c r="AH10" s="98"/>
+      <c r="AI10" s="98"/>
+      <c r="AJ10" s="98"/>
+      <c r="AK10" s="98"/>
+      <c r="AL10" s="97"/>
+      <c r="AM10" s="98"/>
+      <c r="AN10" s="98"/>
+      <c r="AO10" s="98"/>
+      <c r="AP10" s="98"/>
+      <c r="AQ10" s="98"/>
+      <c r="AR10" s="98"/>
+      <c r="AS10" s="98"/>
+      <c r="AT10" s="98"/>
+      <c r="AU10" s="98"/>
+      <c r="AV10" s="98"/>
+      <c r="AW10" s="98"/>
+      <c r="AX10" s="98"/>
+      <c r="AY10" s="98"/>
+      <c r="AZ10" s="98"/>
+      <c r="BA10" s="97"/>
+      <c r="BB10" s="98"/>
+      <c r="BC10" s="98"/>
+      <c r="BD10" s="98"/>
+      <c r="BE10" s="98"/>
+      <c r="BF10" s="98"/>
+      <c r="BG10" s="98"/>
+      <c r="BH10" s="98"/>
+      <c r="BI10" s="98"/>
+      <c r="BJ10" s="98"/>
+      <c r="BK10" s="98"/>
+      <c r="BL10" s="98"/>
+      <c r="BM10" s="98"/>
+      <c r="BN10" s="98"/>
+      <c r="BO10" s="98"/>
+      <c r="BP10" s="98"/>
+      <c r="BQ10" s="98"/>
+      <c r="BR10" s="98"/>
+      <c r="BS10" s="98"/>
+      <c r="BT10" s="98"/>
+      <c r="BU10" s="98"/>
+      <c r="BV10" s="98"/>
+      <c r="BW10" s="98"/>
+      <c r="BX10" s="98"/>
+      <c r="BY10" s="99"/>
     </row>
-    <row r="11" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A11" s="31"/>
-      <c r="B11" s="84"/>
-      <c r="C11" s="84"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="84"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="84"/>
-      <c r="H11" s="97" t="s">
+      <c r="B11" s="93"/>
+      <c r="C11" s="93"/>
+      <c r="D11" s="93"/>
+      <c r="E11" s="93"/>
+      <c r="F11" s="93"/>
+      <c r="G11" s="93"/>
+      <c r="H11" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="98"/>
-      <c r="J11" s="98"/>
-      <c r="K11" s="98"/>
-      <c r="L11" s="99"/>
-      <c r="M11" s="97" t="s">
+      <c r="I11" s="95"/>
+      <c r="J11" s="95"/>
+      <c r="K11" s="95"/>
+      <c r="L11" s="96"/>
+      <c r="M11" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="N11" s="98"/>
-      <c r="O11" s="98"/>
-      <c r="P11" s="98"/>
-      <c r="Q11" s="99"/>
-      <c r="R11" s="97" t="s">
+      <c r="N11" s="95"/>
+      <c r="O11" s="95"/>
+      <c r="P11" s="95"/>
+      <c r="Q11" s="96"/>
+      <c r="R11" s="94" t="s">
         <v>34</v>
       </c>
-      <c r="S11" s="98"/>
-      <c r="T11" s="98"/>
-      <c r="U11" s="98"/>
-      <c r="V11" s="99"/>
-      <c r="W11" s="97" t="s">
+      <c r="S11" s="95"/>
+      <c r="T11" s="95"/>
+      <c r="U11" s="95"/>
+      <c r="V11" s="96"/>
+      <c r="W11" s="94" t="s">
         <v>23</v>
       </c>
-      <c r="X11" s="98"/>
-      <c r="Y11" s="98"/>
-      <c r="Z11" s="98"/>
-      <c r="AA11" s="99"/>
-      <c r="AB11" s="97" t="s">
+      <c r="X11" s="95"/>
+      <c r="Y11" s="95"/>
+      <c r="Z11" s="95"/>
+      <c r="AA11" s="96"/>
+      <c r="AB11" s="94" t="s">
         <v>33</v>
       </c>
-      <c r="AC11" s="98"/>
-      <c r="AD11" s="98"/>
-      <c r="AE11" s="98"/>
-      <c r="AF11" s="99"/>
-      <c r="AG11" s="97" t="s">
+      <c r="AC11" s="95"/>
+      <c r="AD11" s="95"/>
+      <c r="AE11" s="95"/>
+      <c r="AF11" s="96"/>
+      <c r="AG11" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="AH11" s="98"/>
-      <c r="AI11" s="98"/>
-      <c r="AJ11" s="98"/>
-      <c r="AK11" s="99"/>
-      <c r="AL11" s="97" t="s">
+      <c r="AH11" s="95"/>
+      <c r="AI11" s="95"/>
+      <c r="AJ11" s="95"/>
+      <c r="AK11" s="96"/>
+      <c r="AL11" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="AM11" s="98"/>
-      <c r="AN11" s="98"/>
-      <c r="AO11" s="98"/>
-      <c r="AP11" s="99"/>
-      <c r="AQ11" s="97" t="s">
+      <c r="AM11" s="95"/>
+      <c r="AN11" s="95"/>
+      <c r="AO11" s="95"/>
+      <c r="AP11" s="96"/>
+      <c r="AQ11" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="AR11" s="98"/>
-      <c r="AS11" s="98"/>
-      <c r="AT11" s="98"/>
-      <c r="AU11" s="99"/>
-      <c r="AV11" s="97" t="s">
+      <c r="AR11" s="95"/>
+      <c r="AS11" s="95"/>
+      <c r="AT11" s="95"/>
+      <c r="AU11" s="96"/>
+      <c r="AV11" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="AW11" s="98"/>
-      <c r="AX11" s="98"/>
-      <c r="AY11" s="98"/>
-      <c r="AZ11" s="99"/>
-      <c r="BA11" s="97" t="s">
+      <c r="AW11" s="95"/>
+      <c r="AX11" s="95"/>
+      <c r="AY11" s="95"/>
+      <c r="AZ11" s="96"/>
+      <c r="BA11" s="94" t="s">
         <v>28</v>
       </c>
-      <c r="BB11" s="98"/>
-      <c r="BC11" s="98"/>
-      <c r="BD11" s="98"/>
-      <c r="BE11" s="99"/>
-      <c r="BF11" s="97" t="s">
+      <c r="BB11" s="95"/>
+      <c r="BC11" s="95"/>
+      <c r="BD11" s="95"/>
+      <c r="BE11" s="96"/>
+      <c r="BF11" s="94" t="s">
         <v>27</v>
       </c>
-      <c r="BG11" s="98"/>
-      <c r="BH11" s="98"/>
-      <c r="BI11" s="98"/>
-      <c r="BJ11" s="99"/>
-      <c r="BK11" s="97" t="s">
+      <c r="BG11" s="95"/>
+      <c r="BH11" s="95"/>
+      <c r="BI11" s="95"/>
+      <c r="BJ11" s="96"/>
+      <c r="BK11" s="94" t="s">
         <v>26</v>
       </c>
-      <c r="BL11" s="98"/>
-      <c r="BM11" s="98"/>
-      <c r="BN11" s="98"/>
-      <c r="BO11" s="99"/>
-      <c r="BP11" s="97" t="s">
+      <c r="BL11" s="95"/>
+      <c r="BM11" s="95"/>
+      <c r="BN11" s="95"/>
+      <c r="BO11" s="96"/>
+      <c r="BP11" s="94" t="s">
         <v>25</v>
       </c>
-      <c r="BQ11" s="98"/>
-      <c r="BR11" s="98"/>
-      <c r="BS11" s="98"/>
-      <c r="BT11" s="99"/>
-      <c r="BU11" s="97" t="s">
+      <c r="BQ11" s="95"/>
+      <c r="BR11" s="95"/>
+      <c r="BS11" s="95"/>
+      <c r="BT11" s="96"/>
+      <c r="BU11" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="BV11" s="98"/>
-      <c r="BW11" s="98"/>
-      <c r="BX11" s="98"/>
-      <c r="BY11" s="99"/>
+      <c r="BV11" s="95"/>
+      <c r="BW11" s="95"/>
+      <c r="BX11" s="95"/>
+      <c r="BY11" s="96"/>
     </row>
-    <row r="12" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A12" s="31"/>
       <c r="B12" s="24">
         <v>1</v>
@@ -2428,7 +2431,7 @@
       <c r="BX12" s="30"/>
       <c r="BY12" s="30"/>
     </row>
-    <row r="13" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A13" s="31"/>
       <c r="B13" s="32">
         <v>1.1000000000000001</v>
@@ -2520,7 +2523,7 @@
       <c r="BX13" s="36"/>
       <c r="BY13" s="36"/>
     </row>
-    <row r="14" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A14" s="31"/>
       <c r="B14" s="32">
         <v>1.2</v>
@@ -2612,7 +2615,7 @@
       <c r="BX14" s="51"/>
       <c r="BY14" s="51"/>
     </row>
-    <row r="15" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A15" s="31"/>
       <c r="B15" s="32">
         <v>1.3</v>
@@ -2704,7 +2707,7 @@
       <c r="BX15" s="51"/>
       <c r="BY15" s="51"/>
     </row>
-    <row r="16" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A16" s="31"/>
       <c r="B16" s="32">
         <v>1.4</v>
@@ -2796,7 +2799,7 @@
       <c r="BX16" s="51"/>
       <c r="BY16" s="51"/>
     </row>
-    <row r="17" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A17" s="31"/>
       <c r="B17" s="32">
         <v>1.5</v>
@@ -2888,7 +2891,7 @@
       <c r="BX17" s="36"/>
       <c r="BY17" s="36"/>
     </row>
-    <row r="18" spans="1:77" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:77" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="19"/>
       <c r="B18" s="32">
         <v>1.6</v>
@@ -2972,7 +2975,7 @@
       <c r="BX18" s="36"/>
       <c r="BY18" s="36"/>
     </row>
-    <row r="19" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A19" s="31"/>
       <c r="B19" s="32">
         <v>1.7</v>
@@ -3056,7 +3059,7 @@
       <c r="BX19" s="36"/>
       <c r="BY19" s="36"/>
     </row>
-    <row r="20" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A20" s="31"/>
       <c r="B20" s="24">
         <v>2</v>
@@ -3139,7 +3142,7 @@
       <c r="BX20" s="30"/>
       <c r="BY20" s="30"/>
     </row>
-    <row r="21" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A21" s="31"/>
       <c r="B21" s="32">
         <v>2.1</v>
@@ -3228,7 +3231,7 @@
       <c r="BX21" s="36"/>
       <c r="BY21" s="36"/>
     </row>
-    <row r="22" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A22" s="31"/>
       <c r="B22" s="32">
         <v>2.2000000000000002</v>
@@ -3318,7 +3321,7 @@
       <c r="BX22" s="36"/>
       <c r="BY22" s="36"/>
     </row>
-    <row r="23" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A23" s="31"/>
       <c r="B23" s="32">
         <v>2.2999999999999998</v>
@@ -3357,15 +3360,15 @@
       <c r="Y23" s="72"/>
       <c r="Z23" s="72"/>
       <c r="AA23" s="72"/>
-      <c r="AB23" s="108"/>
-      <c r="AC23" s="108"/>
-      <c r="AD23" s="108"/>
-      <c r="AE23" s="108"/>
-      <c r="AF23" s="108"/>
+      <c r="AB23" s="84"/>
+      <c r="AC23" s="84"/>
+      <c r="AD23" s="84"/>
+      <c r="AE23" s="84"/>
+      <c r="AF23" s="84"/>
       <c r="AG23" s="72"/>
       <c r="AH23" s="72"/>
-      <c r="AI23" s="109"/>
-      <c r="AJ23" s="109"/>
+      <c r="AI23" s="85"/>
+      <c r="AJ23" s="85"/>
       <c r="AK23" s="44"/>
       <c r="AL23" s="44"/>
       <c r="AM23" s="44"/>
@@ -3408,7 +3411,7 @@
       <c r="BX23" s="36"/>
       <c r="BY23" s="36"/>
     </row>
-    <row r="24" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A24" s="31"/>
       <c r="B24" s="46"/>
       <c r="C24" s="79" t="s">
@@ -3442,15 +3445,15 @@
       <c r="Y24" s="72"/>
       <c r="Z24" s="72"/>
       <c r="AA24" s="72"/>
-      <c r="AB24" s="108"/>
-      <c r="AC24" s="108"/>
-      <c r="AD24" s="108"/>
-      <c r="AE24" s="108"/>
-      <c r="AF24" s="108"/>
+      <c r="AB24" s="84"/>
+      <c r="AC24" s="84"/>
+      <c r="AD24" s="84"/>
+      <c r="AE24" s="84"/>
+      <c r="AF24" s="84"/>
       <c r="AG24" s="72"/>
       <c r="AH24" s="72"/>
-      <c r="AI24" s="109"/>
-      <c r="AJ24" s="109"/>
+      <c r="AI24" s="85"/>
+      <c r="AJ24" s="85"/>
       <c r="AK24" s="44"/>
       <c r="AL24" s="44"/>
       <c r="AM24" s="44"/>
@@ -3493,7 +3496,7 @@
       <c r="BX24" s="42"/>
       <c r="BY24" s="42"/>
     </row>
-    <row r="25" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A25" s="31"/>
       <c r="B25" s="46"/>
       <c r="C25" s="79" t="s">
@@ -3527,15 +3530,15 @@
       <c r="Y25" s="72"/>
       <c r="Z25" s="72"/>
       <c r="AA25" s="72"/>
-      <c r="AB25" s="108"/>
-      <c r="AC25" s="108"/>
-      <c r="AD25" s="108"/>
-      <c r="AE25" s="108"/>
-      <c r="AF25" s="108"/>
+      <c r="AB25" s="84"/>
+      <c r="AC25" s="84"/>
+      <c r="AD25" s="84"/>
+      <c r="AE25" s="84"/>
+      <c r="AF25" s="84"/>
       <c r="AG25" s="72"/>
       <c r="AH25" s="72"/>
-      <c r="AI25" s="109"/>
-      <c r="AJ25" s="109"/>
+      <c r="AI25" s="85"/>
+      <c r="AJ25" s="85"/>
       <c r="AK25" s="44"/>
       <c r="AL25" s="44"/>
       <c r="AM25" s="44"/>
@@ -3578,7 +3581,7 @@
       <c r="BX25" s="42"/>
       <c r="BY25" s="42"/>
     </row>
-    <row r="26" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A26" s="31"/>
       <c r="B26" s="32">
         <v>2.2999999999999998</v>
@@ -3669,7 +3672,7 @@
       <c r="BX26" s="36"/>
       <c r="BY26" s="36"/>
     </row>
-    <row r="27" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A27" s="31"/>
       <c r="B27" s="32">
         <v>2.4</v>
@@ -3759,7 +3762,7 @@
       <c r="BX27" s="36"/>
       <c r="BY27" s="36"/>
     </row>
-    <row r="28" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A28" s="31"/>
       <c r="B28" s="32">
         <v>2.5</v>
@@ -3848,7 +3851,7 @@
       <c r="BX28" s="36"/>
       <c r="BY28" s="36"/>
     </row>
-    <row r="29" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A29" s="31"/>
       <c r="B29" s="32">
         <v>2.6</v>
@@ -3871,7 +3874,7 @@
       <c r="I29" s="41"/>
       <c r="J29" s="42"/>
       <c r="K29" s="42"/>
-      <c r="L29" s="107"/>
+      <c r="L29" s="83"/>
       <c r="M29" s="43"/>
       <c r="N29" s="43"/>
       <c r="O29" s="43"/>
@@ -3889,13 +3892,13 @@
       <c r="AA29" s="36"/>
       <c r="AB29" s="37"/>
       <c r="AC29" s="37"/>
-      <c r="AD29" s="108"/>
-      <c r="AE29" s="108"/>
-      <c r="AF29" s="108"/>
+      <c r="AD29" s="84"/>
+      <c r="AE29" s="84"/>
+      <c r="AF29" s="84"/>
       <c r="AG29" s="72"/>
       <c r="AH29" s="72"/>
-      <c r="AI29" s="109"/>
-      <c r="AJ29" s="109"/>
+      <c r="AI29" s="85"/>
+      <c r="AJ29" s="85"/>
       <c r="AK29" s="44"/>
       <c r="AL29" s="44"/>
       <c r="AM29" s="44"/>
@@ -3938,7 +3941,7 @@
       <c r="BX29" s="36"/>
       <c r="BY29" s="36"/>
     </row>
-    <row r="30" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A30" s="31"/>
       <c r="B30" s="32">
         <v>2.7</v>
@@ -4024,202 +4027,200 @@
       <c r="BX30" s="36"/>
       <c r="BY30" s="36"/>
     </row>
-    <row r="31" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A31" s="31"/>
-      <c r="B31" s="24">
+      <c r="B31" s="46">
+        <v>2.8</v>
+      </c>
+      <c r="C31" s="50" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="61" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" s="47">
+        <v>44632</v>
+      </c>
+      <c r="F31" s="47"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="41"/>
+      <c r="J31" s="42"/>
+      <c r="K31" s="42"/>
+      <c r="L31" s="45"/>
+      <c r="M31" s="45"/>
+      <c r="N31" s="45"/>
+      <c r="O31" s="45"/>
+      <c r="P31" s="45"/>
+      <c r="Q31" s="45"/>
+      <c r="R31" s="42"/>
+      <c r="S31" s="42"/>
+      <c r="T31" s="42"/>
+      <c r="U31" s="42"/>
+      <c r="V31" s="42"/>
+      <c r="W31" s="42"/>
+      <c r="X31" s="42"/>
+      <c r="Y31" s="42"/>
+      <c r="Z31" s="42"/>
+      <c r="AA31" s="42"/>
+      <c r="AB31" s="37"/>
+      <c r="AC31" s="37"/>
+      <c r="AD31" s="37"/>
+      <c r="AE31" s="37"/>
+      <c r="AF31" s="37"/>
+      <c r="AG31" s="42"/>
+      <c r="AH31" s="42"/>
+      <c r="AI31" s="44"/>
+      <c r="AJ31" s="44"/>
+      <c r="AK31" s="44"/>
+      <c r="AL31" s="85"/>
+      <c r="AM31" s="44"/>
+      <c r="AN31" s="44"/>
+      <c r="AO31" s="44"/>
+      <c r="AP31" s="44"/>
+      <c r="AQ31" s="38"/>
+      <c r="AR31" s="38"/>
+      <c r="AS31" s="38"/>
+      <c r="AT31" s="38"/>
+      <c r="AU31" s="38"/>
+      <c r="AV31" s="42"/>
+      <c r="AW31" s="42"/>
+      <c r="AX31" s="42"/>
+      <c r="AY31" s="42"/>
+      <c r="AZ31" s="42"/>
+      <c r="BA31" s="42"/>
+      <c r="BB31" s="42"/>
+      <c r="BC31" s="42"/>
+      <c r="BD31" s="42"/>
+      <c r="BE31" s="42"/>
+      <c r="BF31" s="39"/>
+      <c r="BG31" s="39"/>
+      <c r="BH31" s="39"/>
+      <c r="BI31" s="39"/>
+      <c r="BJ31" s="39"/>
+      <c r="BK31" s="42"/>
+      <c r="BL31" s="42"/>
+      <c r="BM31" s="42"/>
+      <c r="BN31" s="42"/>
+      <c r="BO31" s="42"/>
+      <c r="BP31" s="42"/>
+      <c r="BQ31" s="42"/>
+      <c r="BR31" s="42"/>
+      <c r="BS31" s="42"/>
+      <c r="BT31" s="42"/>
+      <c r="BU31" s="42"/>
+      <c r="BV31" s="42"/>
+      <c r="BW31" s="42"/>
+      <c r="BX31" s="42"/>
+      <c r="BY31" s="42"/>
+    </row>
+    <row r="32" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="31"/>
+      <c r="B32" s="24">
         <v>3</v>
       </c>
-      <c r="C31" s="25" t="s">
+      <c r="C32" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="29"/>
-      <c r="K31" s="29"/>
-      <c r="L31" s="30"/>
-      <c r="M31" s="27"/>
-      <c r="N31" s="30"/>
-      <c r="O31" s="27"/>
-      <c r="P31" s="30"/>
-      <c r="Q31" s="30"/>
-      <c r="R31" s="30"/>
-      <c r="S31" s="30"/>
-      <c r="T31" s="30"/>
-      <c r="U31" s="30"/>
-      <c r="V31" s="30"/>
-      <c r="W31" s="30"/>
-      <c r="X31" s="30"/>
-      <c r="Y31" s="30"/>
-      <c r="Z31" s="30"/>
-      <c r="AA31" s="30"/>
-      <c r="AB31" s="30"/>
-      <c r="AC31" s="30"/>
-      <c r="AD31" s="30"/>
-      <c r="AE31" s="30"/>
-      <c r="AF31" s="30"/>
-      <c r="AG31" s="30"/>
-      <c r="AH31" s="30"/>
-      <c r="AI31" s="30"/>
-      <c r="AJ31" s="30"/>
-      <c r="AK31" s="30"/>
-      <c r="AL31" s="30"/>
-      <c r="AM31" s="30"/>
-      <c r="AN31" s="30"/>
-      <c r="AO31" s="30"/>
-      <c r="AP31" s="30"/>
-      <c r="AQ31" s="30"/>
-      <c r="AR31" s="30"/>
-      <c r="AS31" s="30"/>
-      <c r="AT31" s="30"/>
-      <c r="AU31" s="30"/>
-      <c r="AV31" s="30"/>
-      <c r="AW31" s="30"/>
-      <c r="AX31" s="30"/>
-      <c r="AY31" s="30"/>
-      <c r="AZ31" s="30"/>
-      <c r="BA31" s="30"/>
-      <c r="BB31" s="30"/>
-      <c r="BC31" s="30"/>
-      <c r="BD31" s="30"/>
-      <c r="BE31" s="30"/>
-      <c r="BF31" s="30"/>
-      <c r="BG31" s="30"/>
-      <c r="BH31" s="30"/>
-      <c r="BI31" s="30"/>
-      <c r="BJ31" s="30"/>
-      <c r="BK31" s="30"/>
-      <c r="BL31" s="30"/>
-      <c r="BM31" s="30"/>
-      <c r="BN31" s="30"/>
-      <c r="BO31" s="30"/>
-      <c r="BP31" s="30"/>
-      <c r="BQ31" s="30"/>
-      <c r="BR31" s="30"/>
-      <c r="BS31" s="30"/>
-      <c r="BT31" s="30"/>
-      <c r="BU31" s="30"/>
-      <c r="BV31" s="30"/>
-      <c r="BW31" s="30"/>
-      <c r="BX31" s="30"/>
-      <c r="BY31" s="30"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="29"/>
+      <c r="L32" s="30"/>
+      <c r="M32" s="27"/>
+      <c r="N32" s="30"/>
+      <c r="O32" s="27"/>
+      <c r="P32" s="30"/>
+      <c r="Q32" s="30"/>
+      <c r="R32" s="30"/>
+      <c r="S32" s="30"/>
+      <c r="T32" s="30"/>
+      <c r="U32" s="30"/>
+      <c r="V32" s="30"/>
+      <c r="W32" s="30"/>
+      <c r="X32" s="30"/>
+      <c r="Y32" s="30"/>
+      <c r="Z32" s="30"/>
+      <c r="AA32" s="30"/>
+      <c r="AB32" s="30"/>
+      <c r="AC32" s="30"/>
+      <c r="AD32" s="30"/>
+      <c r="AE32" s="30"/>
+      <c r="AF32" s="30"/>
+      <c r="AG32" s="30"/>
+      <c r="AH32" s="30"/>
+      <c r="AI32" s="30"/>
+      <c r="AJ32" s="30"/>
+      <c r="AK32" s="30"/>
+      <c r="AL32" s="30"/>
+      <c r="AM32" s="30"/>
+      <c r="AN32" s="30"/>
+      <c r="AO32" s="30"/>
+      <c r="AP32" s="30"/>
+      <c r="AQ32" s="30"/>
+      <c r="AR32" s="30"/>
+      <c r="AS32" s="30"/>
+      <c r="AT32" s="30"/>
+      <c r="AU32" s="30"/>
+      <c r="AV32" s="30"/>
+      <c r="AW32" s="30"/>
+      <c r="AX32" s="30"/>
+      <c r="AY32" s="30"/>
+      <c r="AZ32" s="30"/>
+      <c r="BA32" s="30"/>
+      <c r="BB32" s="30"/>
+      <c r="BC32" s="30"/>
+      <c r="BD32" s="30"/>
+      <c r="BE32" s="30"/>
+      <c r="BF32" s="30"/>
+      <c r="BG32" s="30"/>
+      <c r="BH32" s="30"/>
+      <c r="BI32" s="30"/>
+      <c r="BJ32" s="30"/>
+      <c r="BK32" s="30"/>
+      <c r="BL32" s="30"/>
+      <c r="BM32" s="30"/>
+      <c r="BN32" s="30"/>
+      <c r="BO32" s="30"/>
+      <c r="BP32" s="30"/>
+      <c r="BQ32" s="30"/>
+      <c r="BR32" s="30"/>
+      <c r="BS32" s="30"/>
+      <c r="BT32" s="30"/>
+      <c r="BU32" s="30"/>
+      <c r="BV32" s="30"/>
+      <c r="BW32" s="30"/>
+      <c r="BX32" s="30"/>
+      <c r="BY32" s="30"/>
     </row>
-    <row r="32" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
-      <c r="B32" s="32">
-        <v>3.1</v>
-      </c>
-      <c r="C32" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="D32" s="63" t="s">
-        <v>48</v>
-      </c>
-      <c r="E32" s="34">
-        <v>44595</v>
-      </c>
-      <c r="F32" s="34"/>
-      <c r="G32" s="35">
-        <f>DAYS360(E32,F32)</f>
-        <v>-43953</v>
-      </c>
-      <c r="H32" s="40"/>
-      <c r="I32" s="41"/>
-      <c r="J32" s="42"/>
-      <c r="K32" s="72"/>
-      <c r="L32" s="72"/>
-      <c r="M32" s="75"/>
-      <c r="N32" s="75"/>
-      <c r="O32" s="75"/>
-      <c r="P32" s="75"/>
-      <c r="Q32" s="75"/>
-      <c r="R32" s="72"/>
-      <c r="S32" s="72"/>
-      <c r="T32" s="72"/>
-      <c r="U32" s="72"/>
-      <c r="V32" s="72"/>
-      <c r="W32" s="72"/>
-      <c r="X32" s="72"/>
-      <c r="Y32" s="72"/>
-      <c r="Z32" s="72"/>
-      <c r="AA32" s="72"/>
-      <c r="AB32" s="108"/>
-      <c r="AC32" s="108"/>
-      <c r="AD32" s="108"/>
-      <c r="AE32" s="108"/>
-      <c r="AF32" s="108"/>
-      <c r="AG32" s="72"/>
-      <c r="AH32" s="72"/>
-      <c r="AI32" s="72"/>
-      <c r="AJ32" s="72"/>
-      <c r="AK32" s="42"/>
-      <c r="AL32" s="42"/>
-      <c r="AM32" s="42"/>
-      <c r="AN32" s="42"/>
-      <c r="AO32" s="42"/>
-      <c r="AP32" s="42"/>
-      <c r="AQ32" s="38"/>
-      <c r="AR32" s="38"/>
-      <c r="AS32" s="38"/>
-      <c r="AT32" s="38"/>
-      <c r="AU32" s="38"/>
-      <c r="AV32" s="42"/>
-      <c r="AW32" s="42"/>
-      <c r="AX32" s="42"/>
-      <c r="AY32" s="42"/>
-      <c r="AZ32" s="42"/>
-      <c r="BA32" s="42"/>
-      <c r="BB32" s="42"/>
-      <c r="BC32" s="42"/>
-      <c r="BD32" s="42"/>
-      <c r="BE32" s="42"/>
-      <c r="BF32" s="39"/>
-      <c r="BG32" s="39"/>
-      <c r="BH32" s="39"/>
-      <c r="BI32" s="39"/>
-      <c r="BJ32" s="39"/>
-      <c r="BK32" s="36"/>
-      <c r="BL32" s="36"/>
-      <c r="BM32" s="36"/>
-      <c r="BN32" s="36"/>
-      <c r="BO32" s="36"/>
-      <c r="BP32" s="36"/>
-      <c r="BQ32" s="36"/>
-      <c r="BR32" s="36"/>
-      <c r="BS32" s="36"/>
-      <c r="BT32" s="36"/>
-      <c r="BU32" s="36"/>
-      <c r="BV32" s="36"/>
-      <c r="BW32" s="36"/>
-      <c r="BX32" s="36"/>
-      <c r="BY32" s="36"/>
-    </row>
-    <row r="33" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A33" s="31"/>
       <c r="B33" s="32">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="C33" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="D33" s="70" t="s">
-        <v>55</v>
+        <v>67</v>
+      </c>
+      <c r="D33" s="63" t="s">
+        <v>48</v>
       </c>
       <c r="E33" s="34">
-        <v>44596</v>
+        <v>44595</v>
       </c>
       <c r="F33" s="34"/>
       <c r="G33" s="35">
-        <v>0</v>
+        <f>DAYS360(E33,F33)</f>
+        <v>-43953</v>
       </c>
       <c r="H33" s="40"/>
       <c r="I33" s="41"/>
       <c r="J33" s="42"/>
-      <c r="K33" s="42"/>
-      <c r="L33" s="73"/>
+      <c r="K33" s="72"/>
+      <c r="L33" s="72"/>
       <c r="M33" s="75"/>
       <c r="N33" s="75"/>
       <c r="O33" s="75"/>
@@ -4231,19 +4232,19 @@
       <c r="U33" s="72"/>
       <c r="V33" s="72"/>
       <c r="W33" s="72"/>
-      <c r="X33" s="57"/>
-      <c r="Y33" s="36"/>
-      <c r="Z33" s="36"/>
-      <c r="AA33" s="36"/>
-      <c r="AB33" s="37"/>
-      <c r="AC33" s="37"/>
-      <c r="AD33" s="37"/>
-      <c r="AE33" s="37"/>
-      <c r="AF33" s="37"/>
-      <c r="AG33" s="36"/>
-      <c r="AH33" s="36"/>
-      <c r="AI33" s="42"/>
-      <c r="AJ33" s="42"/>
+      <c r="X33" s="72"/>
+      <c r="Y33" s="72"/>
+      <c r="Z33" s="72"/>
+      <c r="AA33" s="72"/>
+      <c r="AB33" s="84"/>
+      <c r="AC33" s="84"/>
+      <c r="AD33" s="84"/>
+      <c r="AE33" s="84"/>
+      <c r="AF33" s="84"/>
+      <c r="AG33" s="72"/>
+      <c r="AH33" s="72"/>
+      <c r="AI33" s="72"/>
+      <c r="AJ33" s="72"/>
       <c r="AK33" s="42"/>
       <c r="AL33" s="42"/>
       <c r="AM33" s="42"/>
@@ -4286,60 +4287,59 @@
       <c r="BX33" s="36"/>
       <c r="BY33" s="36"/>
     </row>
-    <row r="34" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A34" s="31"/>
       <c r="B34" s="32">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="C34" s="50" t="s">
-        <v>60</v>
-      </c>
-      <c r="D34" s="69" t="s">
-        <v>52</v>
+        <v>41</v>
+      </c>
+      <c r="D34" s="70" t="s">
+        <v>55</v>
       </c>
       <c r="E34" s="34">
-        <v>44606</v>
+        <v>44596</v>
       </c>
       <c r="F34" s="34"/>
       <c r="G34" s="35">
-        <f t="shared" ref="G34:G36" si="4">DAYS360(E34,F34)</f>
-        <v>-43964</v>
+        <v>0</v>
       </c>
       <c r="H34" s="40"/>
       <c r="I34" s="41"/>
       <c r="J34" s="42"/>
       <c r="K34" s="42"/>
-      <c r="L34" s="36"/>
-      <c r="M34" s="43"/>
-      <c r="N34" s="43"/>
-      <c r="O34" s="43"/>
-      <c r="P34" s="43"/>
-      <c r="Q34" s="43"/>
+      <c r="L34" s="73"/>
+      <c r="M34" s="75"/>
+      <c r="N34" s="75"/>
+      <c r="O34" s="75"/>
+      <c r="P34" s="75"/>
+      <c r="Q34" s="75"/>
       <c r="R34" s="72"/>
       <c r="S34" s="72"/>
       <c r="T34" s="72"/>
       <c r="U34" s="72"/>
       <c r="V34" s="72"/>
       <c r="W34" s="72"/>
-      <c r="X34" s="72"/>
-      <c r="Y34" s="72"/>
-      <c r="Z34" s="72"/>
-      <c r="AA34" s="72"/>
-      <c r="AB34" s="108"/>
-      <c r="AC34" s="108"/>
-      <c r="AD34" s="108"/>
-      <c r="AE34" s="108"/>
-      <c r="AF34" s="108"/>
-      <c r="AG34" s="72"/>
-      <c r="AH34" s="72"/>
-      <c r="AI34" s="72"/>
-      <c r="AJ34" s="72"/>
-      <c r="AK34" s="36"/>
-      <c r="AL34" s="36"/>
-      <c r="AM34" s="36"/>
-      <c r="AN34" s="36"/>
-      <c r="AO34" s="36"/>
-      <c r="AP34" s="36"/>
+      <c r="X34" s="57"/>
+      <c r="Y34" s="36"/>
+      <c r="Z34" s="36"/>
+      <c r="AA34" s="36"/>
+      <c r="AB34" s="37"/>
+      <c r="AC34" s="37"/>
+      <c r="AD34" s="37"/>
+      <c r="AE34" s="37"/>
+      <c r="AF34" s="37"/>
+      <c r="AG34" s="36"/>
+      <c r="AH34" s="36"/>
+      <c r="AI34" s="42"/>
+      <c r="AJ34" s="42"/>
+      <c r="AK34" s="42"/>
+      <c r="AL34" s="42"/>
+      <c r="AM34" s="42"/>
+      <c r="AN34" s="42"/>
+      <c r="AO34" s="42"/>
+      <c r="AP34" s="42"/>
       <c r="AQ34" s="38"/>
       <c r="AR34" s="38"/>
       <c r="AS34" s="38"/>
@@ -4376,54 +4376,54 @@
       <c r="BX34" s="36"/>
       <c r="BY34" s="36"/>
     </row>
-    <row r="35" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A35" s="31"/>
       <c r="B35" s="32">
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
       <c r="C35" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="D35" s="70" t="s">
-        <v>55</v>
+        <v>60</v>
+      </c>
+      <c r="D35" s="69" t="s">
+        <v>52</v>
       </c>
       <c r="E35" s="34">
-        <v>44615</v>
+        <v>44606</v>
       </c>
       <c r="F35" s="34"/>
       <c r="G35" s="35">
-        <f t="shared" si="4"/>
-        <v>-43973</v>
+        <f t="shared" ref="G35:G37" si="4">DAYS360(E35,F35)</f>
+        <v>-43964</v>
       </c>
       <c r="H35" s="40"/>
       <c r="I35" s="41"/>
       <c r="J35" s="42"/>
       <c r="K35" s="42"/>
-      <c r="L35" s="76"/>
+      <c r="L35" s="36"/>
       <c r="M35" s="43"/>
       <c r="N35" s="43"/>
       <c r="O35" s="43"/>
       <c r="P35" s="43"/>
       <c r="Q35" s="43"/>
-      <c r="R35" s="42"/>
-      <c r="S35" s="42"/>
-      <c r="T35" s="42"/>
-      <c r="U35" s="42"/>
-      <c r="V35" s="36"/>
-      <c r="W35" s="36"/>
-      <c r="X35" s="36"/>
-      <c r="Y35" s="110"/>
-      <c r="Z35" s="107"/>
-      <c r="AA35" s="36"/>
-      <c r="AB35" s="37"/>
-      <c r="AC35" s="37"/>
-      <c r="AD35" s="37"/>
-      <c r="AE35" s="37"/>
-      <c r="AF35" s="37"/>
-      <c r="AG35" s="36"/>
-      <c r="AH35" s="36"/>
-      <c r="AI35" s="36"/>
-      <c r="AJ35" s="36"/>
+      <c r="R35" s="72"/>
+      <c r="S35" s="72"/>
+      <c r="T35" s="72"/>
+      <c r="U35" s="72"/>
+      <c r="V35" s="72"/>
+      <c r="W35" s="72"/>
+      <c r="X35" s="72"/>
+      <c r="Y35" s="72"/>
+      <c r="Z35" s="72"/>
+      <c r="AA35" s="72"/>
+      <c r="AB35" s="84"/>
+      <c r="AC35" s="84"/>
+      <c r="AD35" s="84"/>
+      <c r="AE35" s="84"/>
+      <c r="AF35" s="84"/>
+      <c r="AG35" s="72"/>
+      <c r="AH35" s="72"/>
+      <c r="AI35" s="72"/>
+      <c r="AJ35" s="72"/>
       <c r="AK35" s="36"/>
       <c r="AL35" s="36"/>
       <c r="AM35" s="36"/>
@@ -4450,14 +4450,14 @@
       <c r="BH35" s="39"/>
       <c r="BI35" s="39"/>
       <c r="BJ35" s="39"/>
-      <c r="BK35" s="42"/>
-      <c r="BL35" s="42"/>
-      <c r="BM35" s="42"/>
-      <c r="BN35" s="42"/>
-      <c r="BO35" s="42"/>
-      <c r="BP35" s="42"/>
-      <c r="BQ35" s="42"/>
-      <c r="BR35" s="42"/>
+      <c r="BK35" s="36"/>
+      <c r="BL35" s="36"/>
+      <c r="BM35" s="36"/>
+      <c r="BN35" s="36"/>
+      <c r="BO35" s="36"/>
+      <c r="BP35" s="36"/>
+      <c r="BQ35" s="36"/>
+      <c r="BR35" s="36"/>
       <c r="BS35" s="36"/>
       <c r="BT35" s="36"/>
       <c r="BU35" s="36"/>
@@ -4466,29 +4466,30 @@
       <c r="BX35" s="36"/>
       <c r="BY35" s="36"/>
     </row>
-    <row r="36" spans="1:77" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:77" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="31"/>
       <c r="B36" s="32">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="C36" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="D36" s="33" t="s">
-        <v>58</v>
+        <v>43</v>
+      </c>
+      <c r="D36" s="70" t="s">
+        <v>55</v>
       </c>
       <c r="E36" s="34">
-        <v>44609</v>
+        <v>44615</v>
       </c>
       <c r="F36" s="34"/>
       <c r="G36" s="35">
         <f t="shared" si="4"/>
-        <v>-43967</v>
+        <v>-43973</v>
       </c>
       <c r="H36" s="40"/>
       <c r="I36" s="41"/>
       <c r="J36" s="42"/>
       <c r="K36" s="42"/>
-      <c r="L36" s="36"/>
+      <c r="L36" s="76"/>
       <c r="M36" s="43"/>
       <c r="N36" s="43"/>
       <c r="O36" s="43"/>
@@ -4497,22 +4498,22 @@
       <c r="R36" s="42"/>
       <c r="S36" s="42"/>
       <c r="T36" s="42"/>
-      <c r="U36" s="72"/>
-      <c r="V36" s="72"/>
-      <c r="W36" s="72"/>
-      <c r="X36" s="72"/>
-      <c r="Y36" s="72"/>
-      <c r="Z36" s="72"/>
-      <c r="AA36" s="72"/>
-      <c r="AB36" s="108"/>
-      <c r="AC36" s="108"/>
-      <c r="AD36" s="108"/>
-      <c r="AE36" s="108"/>
-      <c r="AF36" s="108"/>
-      <c r="AG36" s="72"/>
-      <c r="AH36" s="72"/>
-      <c r="AI36" s="72"/>
-      <c r="AJ36" s="72"/>
+      <c r="U36" s="42"/>
+      <c r="V36" s="36"/>
+      <c r="W36" s="36"/>
+      <c r="X36" s="36"/>
+      <c r="Y36" s="86"/>
+      <c r="Z36" s="83"/>
+      <c r="AA36" s="36"/>
+      <c r="AB36" s="37"/>
+      <c r="AC36" s="37"/>
+      <c r="AD36" s="37"/>
+      <c r="AE36" s="37"/>
+      <c r="AF36" s="37"/>
+      <c r="AG36" s="36"/>
+      <c r="AH36" s="36"/>
+      <c r="AI36" s="36"/>
+      <c r="AJ36" s="36"/>
       <c r="AK36" s="36"/>
       <c r="AL36" s="36"/>
       <c r="AM36" s="36"/>
@@ -4524,16 +4525,16 @@
       <c r="AS36" s="38"/>
       <c r="AT36" s="38"/>
       <c r="AU36" s="38"/>
-      <c r="AV36" s="36"/>
-      <c r="AW36" s="36"/>
-      <c r="AX36" s="36"/>
-      <c r="AY36" s="36"/>
-      <c r="AZ36" s="36"/>
-      <c r="BA36" s="36"/>
-      <c r="BB36" s="36"/>
-      <c r="BC36" s="36"/>
-      <c r="BD36" s="36"/>
-      <c r="BE36" s="36"/>
+      <c r="AV36" s="42"/>
+      <c r="AW36" s="42"/>
+      <c r="AX36" s="42"/>
+      <c r="AY36" s="42"/>
+      <c r="AZ36" s="42"/>
+      <c r="BA36" s="42"/>
+      <c r="BB36" s="42"/>
+      <c r="BC36" s="42"/>
+      <c r="BD36" s="42"/>
+      <c r="BE36" s="42"/>
       <c r="BF36" s="39"/>
       <c r="BG36" s="39"/>
       <c r="BH36" s="39"/>
@@ -4555,75 +4556,74 @@
       <c r="BX36" s="36"/>
       <c r="BY36" s="36"/>
     </row>
-    <row r="37" spans="1:77" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="46">
-        <v>3.6</v>
+    <row r="37" spans="1:77" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="32">
+        <v>3.5</v>
       </c>
       <c r="C37" s="50" t="s">
-        <v>53</v>
-      </c>
-      <c r="D37" s="71" t="s">
-        <v>54</v>
-      </c>
-      <c r="E37" s="47">
-        <v>44565</v>
-      </c>
-      <c r="F37" s="47">
-        <v>44614</v>
-      </c>
-      <c r="G37" s="48">
-        <v>0</v>
+        <v>63</v>
+      </c>
+      <c r="D37" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="E37" s="34">
+        <v>44609</v>
+      </c>
+      <c r="F37" s="34"/>
+      <c r="G37" s="35">
+        <f t="shared" si="4"/>
+        <v>-43967</v>
       </c>
       <c r="H37" s="40"/>
       <c r="I37" s="41"/>
       <c r="J37" s="42"/>
       <c r="K37" s="42"/>
-      <c r="L37" s="72"/>
-      <c r="M37" s="75"/>
-      <c r="N37" s="75"/>
-      <c r="O37" s="75"/>
-      <c r="P37" s="75"/>
-      <c r="Q37" s="75"/>
-      <c r="R37" s="72"/>
-      <c r="S37" s="72"/>
-      <c r="T37" s="72"/>
+      <c r="L37" s="36"/>
+      <c r="M37" s="43"/>
+      <c r="N37" s="43"/>
+      <c r="O37" s="43"/>
+      <c r="P37" s="43"/>
+      <c r="Q37" s="43"/>
+      <c r="R37" s="42"/>
+      <c r="S37" s="42"/>
+      <c r="T37" s="42"/>
       <c r="U37" s="72"/>
       <c r="V37" s="72"/>
       <c r="W37" s="72"/>
-      <c r="X37" s="57"/>
-      <c r="Y37" s="51"/>
-      <c r="Z37" s="51"/>
-      <c r="AA37" s="42"/>
-      <c r="AB37" s="37"/>
-      <c r="AC37" s="37"/>
-      <c r="AD37" s="37"/>
-      <c r="AE37" s="37"/>
-      <c r="AF37" s="37"/>
-      <c r="AG37" s="42"/>
-      <c r="AH37" s="42"/>
-      <c r="AI37" s="42"/>
-      <c r="AJ37" s="42"/>
-      <c r="AK37" s="42"/>
-      <c r="AL37" s="42"/>
-      <c r="AM37" s="42"/>
-      <c r="AN37" s="42"/>
-      <c r="AO37" s="42"/>
-      <c r="AP37" s="42"/>
+      <c r="X37" s="72"/>
+      <c r="Y37" s="72"/>
+      <c r="Z37" s="72"/>
+      <c r="AA37" s="72"/>
+      <c r="AB37" s="84"/>
+      <c r="AC37" s="84"/>
+      <c r="AD37" s="84"/>
+      <c r="AE37" s="84"/>
+      <c r="AF37" s="84"/>
+      <c r="AG37" s="72"/>
+      <c r="AH37" s="72"/>
+      <c r="AI37" s="72"/>
+      <c r="AJ37" s="72"/>
+      <c r="AK37" s="36"/>
+      <c r="AL37" s="36"/>
+      <c r="AM37" s="36"/>
+      <c r="AN37" s="36"/>
+      <c r="AO37" s="36"/>
+      <c r="AP37" s="36"/>
       <c r="AQ37" s="38"/>
       <c r="AR37" s="38"/>
       <c r="AS37" s="38"/>
       <c r="AT37" s="38"/>
       <c r="AU37" s="38"/>
-      <c r="AV37" s="42"/>
-      <c r="AW37" s="42"/>
-      <c r="AX37" s="42"/>
-      <c r="AY37" s="42"/>
-      <c r="AZ37" s="42"/>
-      <c r="BA37" s="42"/>
-      <c r="BB37" s="42"/>
-      <c r="BC37" s="42"/>
-      <c r="BD37" s="42"/>
-      <c r="BE37" s="42"/>
+      <c r="AV37" s="36"/>
+      <c r="AW37" s="36"/>
+      <c r="AX37" s="36"/>
+      <c r="AY37" s="36"/>
+      <c r="AZ37" s="36"/>
+      <c r="BA37" s="36"/>
+      <c r="BB37" s="36"/>
+      <c r="BC37" s="36"/>
+      <c r="BD37" s="36"/>
+      <c r="BE37" s="36"/>
       <c r="BF37" s="39"/>
       <c r="BG37" s="39"/>
       <c r="BH37" s="39"/>
@@ -4637,28 +4637,30 @@
       <c r="BP37" s="42"/>
       <c r="BQ37" s="42"/>
       <c r="BR37" s="42"/>
-      <c r="BS37" s="42"/>
-      <c r="BT37" s="42"/>
-      <c r="BU37" s="42"/>
-      <c r="BV37" s="42"/>
-      <c r="BW37" s="42"/>
-      <c r="BX37" s="42"/>
-      <c r="BY37" s="42"/>
+      <c r="BS37" s="36"/>
+      <c r="BT37" s="36"/>
+      <c r="BU37" s="36"/>
+      <c r="BV37" s="36"/>
+      <c r="BW37" s="36"/>
+      <c r="BX37" s="36"/>
+      <c r="BY37" s="36"/>
     </row>
-    <row r="38" spans="1:77" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:77" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="46">
-        <v>3.7</v>
+        <v>3.6</v>
       </c>
       <c r="C38" s="50" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D38" s="71" t="s">
         <v>54</v>
       </c>
       <c r="E38" s="47">
-        <v>44615</v>
-      </c>
-      <c r="F38" s="47"/>
+        <v>44565</v>
+      </c>
+      <c r="F38" s="47">
+        <v>44614</v>
+      </c>
       <c r="G38" s="48">
         <v>0</v>
       </c>
@@ -4666,31 +4668,31 @@
       <c r="I38" s="41"/>
       <c r="J38" s="42"/>
       <c r="K38" s="42"/>
-      <c r="L38" s="51"/>
-      <c r="M38" s="51"/>
-      <c r="N38" s="51"/>
-      <c r="O38" s="51"/>
-      <c r="P38" s="51"/>
-      <c r="Q38" s="51"/>
-      <c r="R38" s="51"/>
-      <c r="S38" s="51"/>
-      <c r="T38" s="51"/>
-      <c r="U38" s="51"/>
-      <c r="V38" s="51"/>
-      <c r="W38" s="51"/>
-      <c r="X38" s="51"/>
-      <c r="Y38" s="78"/>
-      <c r="Z38" s="78"/>
-      <c r="AA38" s="72"/>
-      <c r="AB38" s="108"/>
-      <c r="AC38" s="108"/>
-      <c r="AD38" s="108"/>
-      <c r="AE38" s="108"/>
-      <c r="AF38" s="108"/>
-      <c r="AG38" s="72"/>
-      <c r="AH38" s="72"/>
-      <c r="AI38" s="72"/>
-      <c r="AJ38" s="72"/>
+      <c r="L38" s="72"/>
+      <c r="M38" s="75"/>
+      <c r="N38" s="75"/>
+      <c r="O38" s="75"/>
+      <c r="P38" s="75"/>
+      <c r="Q38" s="75"/>
+      <c r="R38" s="72"/>
+      <c r="S38" s="72"/>
+      <c r="T38" s="72"/>
+      <c r="U38" s="72"/>
+      <c r="V38" s="72"/>
+      <c r="W38" s="72"/>
+      <c r="X38" s="57"/>
+      <c r="Y38" s="51"/>
+      <c r="Z38" s="51"/>
+      <c r="AA38" s="42"/>
+      <c r="AB38" s="37"/>
+      <c r="AC38" s="37"/>
+      <c r="AD38" s="37"/>
+      <c r="AE38" s="37"/>
+      <c r="AF38" s="37"/>
+      <c r="AG38" s="42"/>
+      <c r="AH38" s="42"/>
+      <c r="AI38" s="42"/>
+      <c r="AJ38" s="42"/>
       <c r="AK38" s="42"/>
       <c r="AL38" s="42"/>
       <c r="AM38" s="42"/>
@@ -4733,18 +4735,105 @@
       <c r="BX38" s="42"/>
       <c r="BY38" s="42"/>
     </row>
+    <row r="39" spans="1:77" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="46">
+        <v>3.7</v>
+      </c>
+      <c r="C39" s="50" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39" s="71" t="s">
+        <v>54</v>
+      </c>
+      <c r="E39" s="47">
+        <v>44615</v>
+      </c>
+      <c r="F39" s="47"/>
+      <c r="G39" s="48">
+        <v>0</v>
+      </c>
+      <c r="H39" s="40"/>
+      <c r="I39" s="41"/>
+      <c r="J39" s="42"/>
+      <c r="K39" s="42"/>
+      <c r="L39" s="51"/>
+      <c r="M39" s="51"/>
+      <c r="N39" s="51"/>
+      <c r="O39" s="51"/>
+      <c r="P39" s="51"/>
+      <c r="Q39" s="51"/>
+      <c r="R39" s="51"/>
+      <c r="S39" s="51"/>
+      <c r="T39" s="51"/>
+      <c r="U39" s="51"/>
+      <c r="V39" s="51"/>
+      <c r="W39" s="51"/>
+      <c r="X39" s="51"/>
+      <c r="Y39" s="78"/>
+      <c r="Z39" s="78"/>
+      <c r="AA39" s="72"/>
+      <c r="AB39" s="84"/>
+      <c r="AC39" s="84"/>
+      <c r="AD39" s="84"/>
+      <c r="AE39" s="84"/>
+      <c r="AF39" s="84"/>
+      <c r="AG39" s="72"/>
+      <c r="AH39" s="72"/>
+      <c r="AI39" s="72"/>
+      <c r="AJ39" s="72"/>
+      <c r="AK39" s="42"/>
+      <c r="AL39" s="42"/>
+      <c r="AM39" s="42"/>
+      <c r="AN39" s="42"/>
+      <c r="AO39" s="42"/>
+      <c r="AP39" s="42"/>
+      <c r="AQ39" s="38"/>
+      <c r="AR39" s="38"/>
+      <c r="AS39" s="38"/>
+      <c r="AT39" s="38"/>
+      <c r="AU39" s="38"/>
+      <c r="AV39" s="42"/>
+      <c r="AW39" s="42"/>
+      <c r="AX39" s="42"/>
+      <c r="AY39" s="42"/>
+      <c r="AZ39" s="42"/>
+      <c r="BA39" s="42"/>
+      <c r="BB39" s="42"/>
+      <c r="BC39" s="42"/>
+      <c r="BD39" s="42"/>
+      <c r="BE39" s="42"/>
+      <c r="BF39" s="39"/>
+      <c r="BG39" s="39"/>
+      <c r="BH39" s="39"/>
+      <c r="BI39" s="39"/>
+      <c r="BJ39" s="39"/>
+      <c r="BK39" s="42"/>
+      <c r="BL39" s="42"/>
+      <c r="BM39" s="42"/>
+      <c r="BN39" s="42"/>
+      <c r="BO39" s="42"/>
+      <c r="BP39" s="42"/>
+      <c r="BQ39" s="42"/>
+      <c r="BR39" s="42"/>
+      <c r="BS39" s="42"/>
+      <c r="BT39" s="42"/>
+      <c r="BU39" s="42"/>
+      <c r="BV39" s="42"/>
+      <c r="BW39" s="42"/>
+      <c r="BX39" s="42"/>
+      <c r="BY39" s="42"/>
+    </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:N5"/>
-    <mergeCell ref="O5:Z5"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="R11:V11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="P8:U8"/>
+    <mergeCell ref="P7:U7"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="N2:AD2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="H4:N4"/>
+    <mergeCell ref="O4:AA4"/>
     <mergeCell ref="BA10:BY10"/>
     <mergeCell ref="H11:L11"/>
     <mergeCell ref="M11:Q11"/>
@@ -4760,64 +4849,65 @@
     <mergeCell ref="AL11:AP11"/>
     <mergeCell ref="AQ11:AU11"/>
     <mergeCell ref="AV11:AZ11"/>
+    <mergeCell ref="H10:V10"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:N5"/>
+    <mergeCell ref="O5:Z5"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="R11:V11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:V10"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:M2"/>
-    <mergeCell ref="N2:AD2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="H4:N4"/>
-    <mergeCell ref="O4:AA4"/>
     <mergeCell ref="W10:AK10"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="D7:M7"/>
     <mergeCell ref="P6:U6"/>
-    <mergeCell ref="P8:U8"/>
-    <mergeCell ref="P7:U7"/>
   </mergeCells>
-  <conditionalFormatting sqref="D21:D30">
+  <conditionalFormatting sqref="D21:D31">
     <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"Damien"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13:D19 D32:D38">
+  <conditionalFormatting sqref="D13:D19 D33:D39">
     <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"Damien"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13:D19 D32:D38 D21:D30">
+  <conditionalFormatting sqref="D13:D19 D33:D39 D21:D31">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"Tanner"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13:D19 D32:D38 D21:D30">
+  <conditionalFormatting sqref="D13:D19 D33:D39 D21:D31">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"Evan"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13:D19 D32:D38 D21:D30">
+  <conditionalFormatting sqref="D13:D19 D33:D39 D21:D31">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"Alexis"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13:D19 D32:D38 D21:D30">
+  <conditionalFormatting sqref="D13:D19 D33:D39 D21:D31">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"Humza"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13:D19 D32:D38 D21:D30">
+  <conditionalFormatting sqref="D13:D19 D33:D39 D21:D31">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Joseph Terranova"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13:D19 D32:D38 D21:D30">
+  <conditionalFormatting sqref="D13:D19 D33:D39 D21:D31">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Joe Terranova"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13:D19 D32:D38 D21:D30">
+  <conditionalFormatting sqref="D13:D19 D33:D39 D21:D31">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Joe Trotti"</formula>
     </cfRule>
@@ -4834,7 +4924,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$A$1:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>D13:D19 D32:D38 D21:D30</xm:sqref>
+          <xm:sqref>D13:D19 D33:D39 D21:D31</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4848,44 +4938,44 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="68" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="68" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="68" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="68" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="68" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="68" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="68" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="68" t="s">
         <v>36</v>
       </c>
@@ -4896,9 +4986,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5131,27 +5224,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14D564B3-5264-41FC-B8E0-395B567D9994}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F187D4-7552-4664-8374-8AA9CBDA3C6B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d07d918a-d172-4450-8f4a-7b087689ff85"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5176,9 +5257,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F187D4-7552-4664-8374-8AA9CBDA3C6B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14D564B3-5264-41FC-B8E0-395B567D9994}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d07d918a-d172-4450-8f4a-7b087689ff85"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>